<commit_message>
Boceto datamart, informe y script de generación de tuplas
</commit_message>
<xml_diff>
--- a/2. Nuevos atributos y llenado de la BD/Tablas con nuevos atributos.xlsx
+++ b/2. Nuevos atributos y llenado de la BD/Tablas con nuevos atributos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3c2fa6669311d52/Universidad/4º CURSO - 2º CUATRI/TÉCNICAS AVANZADAS DE MANEJO DE INFORMACIÓN/Proyecto TAMI/2. Nuevos atributos y llenado de la BD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="430" documentId="11_AD4D2F04E46CFB4ACB3E200D2550D58E683EDF2A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B7FF29D9-0C2C-4DE1-8089-8696A81B1180}"/>
+  <xr:revisionPtr revIDLastSave="431" documentId="11_AD4D2F04E46CFB4ACB3E200D2550D58E683EDF2A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A505B9F1-2FD5-459D-8497-C3736177045B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
   <si>
     <t>HOTEL</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>NUM_HABITACIONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>PERSONA</t>
@@ -370,7 +373,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +418,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -489,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -518,6 +526,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,10 +544,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -818,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C38" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D32" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
@@ -844,12 +855,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:16">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:16">
       <c r="B4" s="3" t="s">
@@ -937,13 +948,13 @@
       </c>
     </row>
     <row r="8" spans="2:16">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="2:16">
       <c r="B9" s="3" t="s">
@@ -999,13 +1010,13 @@
       </c>
     </row>
     <row r="13" spans="2:16">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="2:16">
       <c r="B14" s="3" t="s">
@@ -1065,13 +1076,13 @@
       <c r="F16" s="4"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="3" t="s">
@@ -1098,10 +1109,10 @@
       <c r="I19" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J19" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="10" t="s">
         <v>49</v>
       </c>
       <c r="L19" s="9" t="s">
@@ -1142,11 +1153,11 @@
       <c r="F21" s="4"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
@@ -1198,11 +1209,11 @@
       <c r="D27" s="3"/>
     </row>
     <row r="30" spans="2:12">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="2:12">
       <c r="B31" s="5" t="s">
@@ -1238,39 +1249,42 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:12">
+    <row r="33" spans="2:13">
       <c r="B33" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-    </row>
-    <row r="36" spans="2:12">
-      <c r="B36" s="10" t="s">
+      <c r="M33" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
-    </row>
-    <row r="37" spans="2:12">
+    </row>
+    <row r="36" spans="2:13">
+      <c r="B36" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="14"/>
+    </row>
+    <row r="37" spans="2:13">
       <c r="B37" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="30">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" ht="30">
       <c r="B38" s="4" t="s">
         <v>16</v>
       </c>
@@ -1278,32 +1292,32 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13">
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="2:12">
-      <c r="B41" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="14"/>
-    </row>
-    <row r="42" spans="2:12">
+    <row r="41" spans="2:13">
+      <c r="B41" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="11"/>
+    </row>
+    <row r="42" spans="2:13">
       <c r="B42" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E42" s="9"/>
     </row>
-    <row r="43" spans="2:12">
+    <row r="43" spans="2:13">
       <c r="B43" s="4" t="s">
         <v>16</v>
       </c>
@@ -1312,54 +1326,54 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="2:12">
-      <c r="B46" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="G46" s="13" t="s">
+    <row r="46" spans="2:13">
+      <c r="B46" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="H46" s="13"/>
-    </row>
-    <row r="47" spans="2:12">
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="G46" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H46" s="15"/>
+    </row>
+    <row r="47" spans="2:13">
       <c r="B47" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L47" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" ht="60">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" ht="60">
       <c r="B48" s="4" t="s">
         <v>16</v>
       </c>
@@ -1370,16 +1384,16 @@
         <v>20</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K48" s="7" t="s">
         <v>20</v>
@@ -1387,40 +1401,40 @@
     </row>
     <row r="49" spans="2:10">
       <c r="B49" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
     <row r="52" spans="2:10">
-      <c r="B52" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
+      <c r="B52" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
     </row>
     <row r="53" spans="2:10">
       <c r="B53" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="60">
@@ -1428,43 +1442,43 @@
         <v>16</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="2:10">
-      <c r="B57" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
+      <c r="B57" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
     </row>
     <row r="58" spans="2:10">
       <c r="B58" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>9</v>
@@ -1475,7 +1489,7 @@
         <v>16</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -1484,44 +1498,44 @@
       </c>
     </row>
     <row r="62" spans="2:10">
-      <c r="B62" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
+      <c r="B62" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
     </row>
     <row r="63" spans="2:10">
       <c r="B63" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="2:10">
@@ -1529,7 +1543,7 @@
         <v>16</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>58</v>
@@ -1545,18 +1559,18 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B52:E52"/>
     <mergeCell ref="B57:E57"/>
     <mergeCell ref="B62:I62"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B36:E36"/>
     <mergeCell ref="G46:H46"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B46:E46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>